<commit_message>
adding USD15; LimitEE constraint tweaks
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_UC_EEP_32_5_Via_GEC.xlsx
+++ b/SuppXLS/Scen_UC_EEP_32_5_Via_GEC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewVEDA\Veda_models\EU_TIMES_Veda2.0\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED889B4-AF56-4FF2-866D-E880A32E20FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7B2ADB-2607-4846-8696-DBAB179C14CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15795" windowHeight="8745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UCT4" sheetId="14" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
   <si>
     <t>UC_N</t>
   </si>
@@ -287,18 +287,12 @@
     <t>-BIOEMHV, -BIOETHA, -OILDSTkt, -BIOSUGFS</t>
   </si>
   <si>
-    <t>TRA_Bunk, NEU*</t>
-  </si>
-  <si>
     <t>-BIOEMHV, -BIOETHA, -BIOOILFS, -BIOSUGFS</t>
   </si>
   <si>
     <t>EXPBIOEMHV</t>
   </si>
   <si>
-    <t>MINREN*,MIN*HT</t>
-  </si>
-  <si>
     <t>IMPBIOETH</t>
   </si>
   <si>
@@ -317,7 +311,10 @@
     <t>ELCNUC*,NUCH2*</t>
   </si>
   <si>
-    <t>*</t>
+    <t>MINREN*,-MIN*AHT,-MIN*GHT</t>
+  </si>
+  <si>
+    <t>NEU*</t>
   </si>
 </sst>
 </file>
@@ -5505,8 +5502,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5623,7 +5620,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="E7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>18</v>
@@ -5651,11 +5648,9 @@
     </row>
     <row r="9" spans="1:16">
       <c r="E9" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="I9" s="6"/>
       <c r="J9" s="4" t="s">
         <v>18</v>
       </c>
@@ -5671,7 +5666,7 @@
         <v>42</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>18</v>
@@ -5688,7 +5683,7 @@
         <v>43</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>18</v>
@@ -5702,7 +5697,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="E12" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="35"/>
@@ -5720,7 +5715,7 @@
     </row>
     <row r="13" spans="1:16" s="10" customFormat="1">
       <c r="E13" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="35"/>
@@ -5737,7 +5732,7 @@
     </row>
     <row r="14" spans="1:16" s="10" customFormat="1">
       <c r="E14" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="35"/>
@@ -5754,7 +5749,7 @@
     </row>
     <row r="15" spans="1:16" s="10" customFormat="1">
       <c r="E15" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="35"/>
@@ -5791,7 +5786,7 @@
     </row>
     <row r="17" spans="2:19" s="10" customFormat="1">
       <c r="E17" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>18</v>
@@ -5806,7 +5801,7 @@
     </row>
     <row r="18" spans="2:19" s="10" customFormat="1">
       <c r="E18" s="10" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>18</v>
@@ -5826,7 +5821,7 @@
         <v>57</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G19" s="30"/>
       <c r="H19" s="30"/>

</xml_diff>